<commit_message>
Calculate PSNR-HVS-M and CR for BPG, Q=26-30, dental images
</commit_message>
<xml_diff>
--- a/Results/result.xlsx
+++ b/Results/result.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AGU,BPG,JPEG2000" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BPG" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>image</t>
   </si>
@@ -53,19 +53,67 @@
     <t>original</t>
   </si>
   <si>
-    <t>goldhill.bmp</t>
-  </si>
-  <si>
-    <t>AGU</t>
-  </si>
-  <si>
-    <t>lenna.bmp</t>
+    <t>dental1_part11.png</t>
   </si>
   <si>
     <t>BPG</t>
   </si>
   <si>
-    <t>JPEG2000</t>
+    <t>dental1_part10.png</t>
+  </si>
+  <si>
+    <t>dental1_part23.png</t>
+  </si>
+  <si>
+    <t>dental1_part33.png</t>
+  </si>
+  <si>
+    <t>dental1_part00.png</t>
+  </si>
+  <si>
+    <t>dental1_part12.png</t>
+  </si>
+  <si>
+    <t>dental1_part21.png</t>
+  </si>
+  <si>
+    <t>dental1_part13.png</t>
+  </si>
+  <si>
+    <t>dental1_part31.png</t>
+  </si>
+  <si>
+    <t>dental1_part22.png</t>
+  </si>
+  <si>
+    <t>dental1_part20.png</t>
+  </si>
+  <si>
+    <t>dental1_part32.png</t>
+  </si>
+  <si>
+    <t>dental2_part12.png</t>
+  </si>
+  <si>
+    <t>dental2_part03.png</t>
+  </si>
+  <si>
+    <t>dental2_part01.png</t>
+  </si>
+  <si>
+    <t>dental2_part00.png</t>
+  </si>
+  <si>
+    <t>dental2_part11.png</t>
+  </si>
+  <si>
+    <t>dental2_part10.png</t>
+  </si>
+  <si>
+    <t>dental2_part13.png</t>
+  </si>
+  <si>
+    <t>dental2_part02.png</t>
   </si>
 </sst>
 </file>
@@ -414,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,31 +519,31 @@
         <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>29.27819061279297</v>
+        <v>12.35703277587891</v>
       </c>
       <c r="E2" t="n">
-        <v>33.46536126977475</v>
+        <v>37.21166162264625</v>
       </c>
       <c r="F2" t="n">
-        <v>45.73446453197005</v>
+        <v>10.28763402986776</v>
       </c>
       <c r="G2" t="n">
-        <v>31.52836762221573</v>
+        <v>38.00764854513655</v>
       </c>
       <c r="H2" t="n">
-        <v>20.12089981034203</v>
+        <v>2.816483884009739</v>
       </c>
       <c r="I2" t="n">
-        <v>35.09432962320589</v>
+        <v>43.6337309033317</v>
       </c>
       <c r="J2" t="n">
-        <v>16.74720500862454</v>
+        <v>7.983432817639176</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9797677860835301</v>
+        <v>0.9886777176114437</v>
       </c>
       <c r="L2" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -512,31 +560,31 @@
         <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>30.34745025634766</v>
+        <v>15.63451385498047</v>
       </c>
       <c r="E3" t="n">
-        <v>33.3095815264331</v>
+        <v>36.18995979182903</v>
       </c>
       <c r="F3" t="n">
-        <v>47.84080514449559</v>
+        <v>13.70895529955514</v>
       </c>
       <c r="G3" t="n">
-        <v>31.33281880797482</v>
+        <v>36.76076000529569</v>
       </c>
       <c r="H3" t="n">
-        <v>21.32280863251234</v>
+        <v>4.273295459088708</v>
       </c>
       <c r="I3" t="n">
-        <v>34.84235951636067</v>
+        <v>41.82317439542451</v>
       </c>
       <c r="J3" t="n">
-        <v>17.4681148797228</v>
+        <v>10.06774713879714</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9788774932929295</v>
+        <v>0.9850690335436467</v>
       </c>
       <c r="L3" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -553,31 +601,31 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>31.49708938598633</v>
+        <v>18.90168380737305</v>
       </c>
       <c r="E4" t="n">
-        <v>33.14809937935729</v>
+        <v>35.36579866976245</v>
       </c>
       <c r="F4" t="n">
-        <v>50.42992702977416</v>
+        <v>17.87259297511918</v>
       </c>
       <c r="G4" t="n">
-        <v>31.1039202111626</v>
+        <v>35.60892795878044</v>
       </c>
       <c r="H4" t="n">
-        <v>22.88618651239213</v>
+        <v>6.241885029692973</v>
       </c>
       <c r="I4" t="n">
-        <v>34.53506927939992</v>
+        <v>40.17764595806422</v>
       </c>
       <c r="J4" t="n">
-        <v>18.16533850737995</v>
+        <v>12.75950352883913</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9780415424227993</v>
+        <v>0.9808847131592918</v>
       </c>
       <c r="L4" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
@@ -594,31 +642,31 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>32.5022087097168</v>
+        <v>21.76368713378906</v>
       </c>
       <c r="E5" t="n">
-        <v>33.01167486109073</v>
+        <v>34.7534788683592</v>
       </c>
       <c r="F5" t="n">
-        <v>52.62983235275279</v>
+        <v>22.45987780508959</v>
       </c>
       <c r="G5" t="n">
-        <v>30.91848374251551</v>
+        <v>34.61672971752786</v>
       </c>
       <c r="H5" t="n">
-        <v>24.22048419153098</v>
+        <v>8.698825090889546</v>
       </c>
       <c r="I5" t="n">
-        <v>34.28897539996128</v>
+        <v>38.73619762387317</v>
       </c>
       <c r="J5" t="n">
-        <v>18.83353689201811</v>
+        <v>15.71700941303435</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9772293935546678</v>
+        <v>0.9765555045690427</v>
       </c>
       <c r="L5" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -635,31 +683,31 @@
         <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>33.63466262817383</v>
+        <v>24.63233947753906</v>
       </c>
       <c r="E6" t="n">
-        <v>32.86293285009555</v>
+        <v>34.21574699579541</v>
       </c>
       <c r="F6" t="n">
-        <v>55.0757542248922</v>
+        <v>28.12835772959436</v>
       </c>
       <c r="G6" t="n">
-        <v>30.72119907637643</v>
+        <v>33.63935984187795</v>
       </c>
       <c r="H6" t="n">
-        <v>25.69699506269272</v>
+        <v>12.04440249798662</v>
       </c>
       <c r="I6" t="n">
-        <v>34.03198019793085</v>
+        <v>37.32295100598613</v>
       </c>
       <c r="J6" t="n">
-        <v>19.56006566184152</v>
+        <v>19.32075471698113</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9762088492951582</v>
+        <v>0.9712857691958111</v>
       </c>
       <c r="L6" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M6" t="b">
         <v>0</v>
@@ -676,31 +724,31 @@
         <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>17.98593902587891</v>
+        <v>11.26805877685547</v>
       </c>
       <c r="E7" t="n">
-        <v>35.58147244089436</v>
+        <v>37.61231257165692</v>
       </c>
       <c r="F7" t="n">
-        <v>31.16771332798845</v>
+        <v>10.51450403531948</v>
       </c>
       <c r="G7" t="n">
-        <v>33.19375420171612</v>
+        <v>37.91291568848322</v>
       </c>
       <c r="H7" t="n">
-        <v>13.99395374847917</v>
+        <v>3.607040415074195</v>
       </c>
       <c r="I7" t="n">
-        <v>36.67139926679346</v>
+        <v>42.55929352470984</v>
       </c>
       <c r="J7" t="n">
-        <v>24.97323044679432</v>
+        <v>10.58568890324665</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9841589409699631</v>
+        <v>0.9869918381062865</v>
       </c>
       <c r="L7" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
@@ -717,31 +765,31 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>18.56882476806641</v>
+        <v>13.60921478271484</v>
       </c>
       <c r="E8" t="n">
-        <v>35.442959430137</v>
+        <v>36.79247292635311</v>
       </c>
       <c r="F8" t="n">
-        <v>32.67827885928276</v>
+        <v>13.5403108951071</v>
       </c>
       <c r="G8" t="n">
-        <v>32.98821186373517</v>
+        <v>36.81451724696083</v>
       </c>
       <c r="H8" t="n">
-        <v>14.84134134068351</v>
+        <v>5.122533135561802</v>
       </c>
       <c r="I8" t="n">
-        <v>36.41607207193638</v>
+        <v>41.03595584513057</v>
       </c>
       <c r="J8" t="n">
-        <v>25.77367023891456</v>
+        <v>13.20292117854445</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9837541906372326</v>
+        <v>0.9836653798301724</v>
       </c>
       <c r="L8" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M8" t="b">
         <v>0</v>
@@ -758,31 +806,31 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>19.17836380004883</v>
+        <v>15.91939544677734</v>
       </c>
       <c r="E9" t="n">
-        <v>35.30268808237712</v>
+        <v>36.11153789872913</v>
       </c>
       <c r="F9" t="n">
-        <v>34.12185174193066</v>
+        <v>17.12388983601499</v>
       </c>
       <c r="G9" t="n">
-        <v>32.80047769220004</v>
+        <v>35.79477935665268</v>
       </c>
       <c r="H9" t="n">
-        <v>15.6763545475119</v>
+        <v>7.091042183513436</v>
       </c>
       <c r="I9" t="n">
-        <v>36.17835283639879</v>
+        <v>39.62370291934972</v>
       </c>
       <c r="J9" t="n">
-        <v>26.60280089303836</v>
+        <v>16.48082484597007</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9831994687966983</v>
+        <v>0.9798319944968272</v>
       </c>
       <c r="L9" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M9" t="b">
         <v>0</v>
@@ -799,31 +847,31 @@
         <v>13</v>
       </c>
       <c r="D10" t="n">
-        <v>19.6963005065918</v>
+        <v>18.13275146484375</v>
       </c>
       <c r="E10" t="n">
-        <v>35.18695699196235</v>
+        <v>35.54616651900167</v>
       </c>
       <c r="F10" t="n">
-        <v>35.31869115544385</v>
+        <v>21.31316027415945</v>
       </c>
       <c r="G10" t="n">
-        <v>32.65075759804413</v>
+        <v>34.84432510033639</v>
       </c>
       <c r="H10" t="n">
-        <v>16.38294650993532</v>
+        <v>9.58634446415236</v>
       </c>
       <c r="I10" t="n">
-        <v>35.98688347575096</v>
+        <v>38.31427330517086</v>
       </c>
       <c r="J10" t="n">
-        <v>27.49281594126901</v>
+        <v>20.40666355285692</v>
       </c>
       <c r="K10" t="n">
-        <v>0.982812574376059</v>
+        <v>0.9754998671801793</v>
       </c>
       <c r="L10" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M10" t="b">
         <v>0</v>
@@ -840,31 +888,31 @@
         <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>20.25830459594727</v>
+        <v>20.60207748413086</v>
       </c>
       <c r="E11" t="n">
-        <v>35.06477264139515</v>
+        <v>34.99169344653978</v>
       </c>
       <c r="F11" t="n">
-        <v>36.68026040928368</v>
+        <v>26.58004843045666</v>
       </c>
       <c r="G11" t="n">
-        <v>32.48647950611653</v>
+        <v>33.8852459294965</v>
       </c>
       <c r="H11" t="n">
-        <v>17.17597655328468</v>
+        <v>12.95314211165966</v>
       </c>
       <c r="I11" t="n">
-        <v>35.78158922289394</v>
+        <v>37.00705230579394</v>
       </c>
       <c r="J11" t="n">
-        <v>28.28790331283047</v>
+        <v>25.79903552799921</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9822655343721517</v>
+        <v>0.9703578927832672</v>
       </c>
       <c r="L11" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -875,37 +923,37 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>16.61564636230469</v>
+        <v>11.62798309326172</v>
       </c>
       <c r="E12" t="n">
-        <v>35.9256312051215</v>
+        <v>37.47575969220198</v>
       </c>
       <c r="F12" t="n">
-        <v>19.50261792659399</v>
+        <v>10.33272915484433</v>
       </c>
       <c r="G12" t="n">
-        <v>35.22987448235583</v>
+        <v>37.98865315210238</v>
       </c>
       <c r="H12" t="n">
-        <v>6.077730706170373</v>
+        <v>2.826373724870205</v>
       </c>
       <c r="I12" t="n">
-        <v>40.2933890754175</v>
+        <v>43.61850773802048</v>
       </c>
       <c r="J12" t="n">
-        <v>11.28374655647383</v>
+        <v>8.461444110906685</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9890275491208752</v>
+        <v>0.9900571427313821</v>
       </c>
       <c r="L12" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>
@@ -916,37 +964,37 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>19.39730072021484</v>
+        <v>14.42771911621094</v>
       </c>
       <c r="E13" t="n">
-        <v>35.25339062065414</v>
+        <v>36.53882682133359</v>
       </c>
       <c r="F13" t="n">
-        <v>24.25612319480675</v>
+        <v>13.54481400849451</v>
       </c>
       <c r="G13" t="n">
-        <v>34.28258971165254</v>
+        <v>36.81307315001056</v>
       </c>
       <c r="H13" t="n">
-        <v>8.301568093873108</v>
+        <v>4.215744652648016</v>
       </c>
       <c r="I13" t="n">
-        <v>38.93920226299873</v>
+        <v>41.88206063052497</v>
       </c>
       <c r="J13" t="n">
-        <v>12.95177865612648</v>
+        <v>10.4485631153095</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9868557037186044</v>
+        <v>0.9873666828610409</v>
       </c>
       <c r="L13" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
@@ -957,37 +1005,37 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>22.79140853881836</v>
+        <v>17.41510009765625</v>
       </c>
       <c r="E14" t="n">
-        <v>34.55309194891861</v>
+        <v>35.72154385850007</v>
       </c>
       <c r="F14" t="n">
-        <v>30.40984312718857</v>
+        <v>17.55468471708581</v>
       </c>
       <c r="G14" t="n">
-        <v>33.30066181078007</v>
+        <v>35.68687326944607</v>
       </c>
       <c r="H14" t="n">
-        <v>11.38313537502551</v>
+        <v>6.092170661363865</v>
       </c>
       <c r="I14" t="n">
-        <v>37.56818460098421</v>
+        <v>40.28308300043292</v>
       </c>
       <c r="J14" t="n">
-        <v>15.10655218117905</v>
+        <v>13.09214403436049</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9841560452159405</v>
+        <v>0.9839700508653986</v>
       </c>
       <c r="L14" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -998,37 +1046,37 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>26.08431243896484</v>
+        <v>20.16817092895508</v>
       </c>
       <c r="E15" t="n">
-        <v>33.96700967304206</v>
+        <v>35.08413847458375</v>
       </c>
       <c r="F15" t="n">
-        <v>36.81261693268382</v>
+        <v>22.00671716354758</v>
       </c>
       <c r="G15" t="n">
-        <v>32.47083669228721</v>
+        <v>34.70525099054736</v>
       </c>
       <c r="H15" t="n">
-        <v>14.90985739890582</v>
+        <v>8.416445465423914</v>
       </c>
       <c r="I15" t="n">
-        <v>36.39606871081212</v>
+        <v>38.87951647121984</v>
       </c>
       <c r="J15" t="n">
-        <v>17.33412682668783</v>
+        <v>16.16177558569667</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9814607006734108</v>
+        <v>0.9805253296878441</v>
       </c>
       <c r="L15" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
@@ -1039,37 +1087,37 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>29.83078002929688</v>
+        <v>22.72605895996094</v>
       </c>
       <c r="E16" t="n">
-        <v>33.38415751220555</v>
+        <v>34.56556231801078</v>
       </c>
       <c r="F16" t="n">
-        <v>44.72665925086083</v>
+        <v>27.15206421423036</v>
       </c>
       <c r="G16" t="n">
-        <v>31.62513900054962</v>
+        <v>33.79277508793068</v>
       </c>
       <c r="H16" t="n">
-        <v>19.38709203789519</v>
+        <v>11.33020692332282</v>
       </c>
       <c r="I16" t="n">
-        <v>35.25567688798284</v>
+        <v>37.588425194214</v>
       </c>
       <c r="J16" t="n">
-        <v>20.06306444206337</v>
+        <v>19.56444510784387</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9783003022004138</v>
+        <v>0.9767958193691674</v>
       </c>
       <c r="L16" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
@@ -1080,37 +1128,37 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" t="n">
-        <v>11.55133819580078</v>
+        <v>8.260086059570312</v>
       </c>
       <c r="E17" t="n">
-        <v>37.50448061714464</v>
+        <v>38.96095788728908</v>
       </c>
       <c r="F17" t="n">
-        <v>16.26176776748119</v>
+        <v>10.02419530550704</v>
       </c>
       <c r="G17" t="n">
-        <v>36.01912606206911</v>
+        <v>38.12030841261935</v>
       </c>
       <c r="H17" t="n">
-        <v>6.345309471209768</v>
+        <v>4.931365047014758</v>
       </c>
       <c r="I17" t="n">
-        <v>40.10627552662378</v>
+        <v>41.20113208258478</v>
       </c>
       <c r="J17" t="n">
-        <v>19.92127061326849</v>
+        <v>24.14960847535698</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9889159820652089</v>
+        <v>0.9851293009316255</v>
       </c>
       <c r="L17" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M17" t="b">
         <v>0</v>
@@ -1121,37 +1169,37 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18" t="n">
-        <v>12.79822158813477</v>
+        <v>9.374355316162109</v>
       </c>
       <c r="E18" t="n">
-        <v>37.05930735604374</v>
+        <v>38.41138950309273</v>
       </c>
       <c r="F18" t="n">
-        <v>18.80562344054101</v>
+        <v>12.37919666570168</v>
       </c>
       <c r="G18" t="n">
-        <v>35.38792625220704</v>
+        <v>37.20387898330245</v>
       </c>
       <c r="H18" t="n">
-        <v>7.583872006502382</v>
+        <v>6.42977905260221</v>
       </c>
       <c r="I18" t="n">
-        <v>39.33189366092068</v>
+        <v>40.04884311409366</v>
       </c>
       <c r="J18" t="n">
-        <v>22.33483854477294</v>
+        <v>30.699613537885</v>
       </c>
       <c r="K18" t="n">
-        <v>0.9878900353927673</v>
+        <v>0.9822974025047454</v>
       </c>
       <c r="L18" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M18" t="b">
         <v>0</v>
@@ -1162,37 +1210,37 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>14.40560150146484</v>
+        <v>10.32726287841797</v>
       </c>
       <c r="E19" t="n">
-        <v>36.54548964040218</v>
+        <v>37.99095128826826</v>
       </c>
       <c r="F19" t="n">
-        <v>22.05698315541527</v>
+        <v>14.81458186407063</v>
       </c>
       <c r="G19" t="n">
-        <v>34.69534249343661</v>
+        <v>36.42390962675162</v>
       </c>
       <c r="H19" t="n">
-        <v>9.178416945638597</v>
+        <v>8.110390643504095</v>
       </c>
       <c r="I19" t="n">
-        <v>38.50312578474932</v>
+        <v>39.04038588009111</v>
       </c>
       <c r="J19" t="n">
-        <v>25.35977556350972</v>
+        <v>38.05807200929152</v>
       </c>
       <c r="K19" t="n">
-        <v>0.9864825109990327</v>
+        <v>0.9794000021895797</v>
       </c>
       <c r="L19" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M19" t="b">
         <v>0</v>
@@ -1203,37 +1251,37 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" t="n">
-        <v>16.06995010375977</v>
+        <v>11.23636627197266</v>
       </c>
       <c r="E20" t="n">
-        <v>36.07065832561034</v>
+        <v>37.62454473404944</v>
       </c>
       <c r="F20" t="n">
-        <v>25.8154952816792</v>
+        <v>17.4811832981659</v>
       </c>
       <c r="G20" t="n">
-        <v>34.01199899273285</v>
+        <v>35.70509534258851</v>
       </c>
       <c r="H20" t="n">
-        <v>11.20918710513597</v>
+        <v>10.0365949778044</v>
       </c>
       <c r="I20" t="n">
-        <v>37.63506242345609</v>
+        <v>38.11493962119498</v>
       </c>
       <c r="J20" t="n">
-        <v>28.41977450130095</v>
+        <v>46.7363166339811</v>
       </c>
       <c r="K20" t="n">
-        <v>0.9849426340049745</v>
+        <v>0.9763930510489712</v>
       </c>
       <c r="L20" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
@@ -1244,37 +1292,37 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D21" t="n">
-        <v>17.91078186035156</v>
+        <v>12.21159744262695</v>
       </c>
       <c r="E21" t="n">
-        <v>35.59965816324025</v>
+        <v>37.26307881596294</v>
       </c>
       <c r="F21" t="n">
-        <v>30.50610292990132</v>
+        <v>20.45597179730139</v>
       </c>
       <c r="G21" t="n">
-        <v>33.28693629598477</v>
+        <v>35.02260244612089</v>
       </c>
       <c r="H21" t="n">
-        <v>13.85943802606115</v>
+        <v>12.22875824125722</v>
       </c>
       <c r="I21" t="n">
-        <v>36.71334740053066</v>
+        <v>37.25698001652535</v>
       </c>
       <c r="J21" t="n">
-        <v>31.97267959507257</v>
+        <v>57.753690240141</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9831836984219159</v>
+        <v>0.9731900701758263</v>
       </c>
       <c r="L21" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -1285,37 +1333,37 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" t="n">
-        <v>59.58346939086914</v>
+        <v>11.35068511962891</v>
       </c>
       <c r="E22" t="n">
-        <v>30.37954573411469</v>
+        <v>37.58058284828255</v>
       </c>
       <c r="F22" t="n">
-        <v>117.5365529216421</v>
+        <v>10.4300612369202</v>
       </c>
       <c r="G22" t="n">
-        <v>27.42907411166932</v>
+        <v>37.94793502606436</v>
       </c>
       <c r="H22" t="n">
-        <v>69.19108920082458</v>
+        <v>3.379143680533923</v>
       </c>
       <c r="I22" t="n">
-        <v>29.73030193580148</v>
+        <v>42.84273702583275</v>
       </c>
       <c r="J22" t="n">
-        <v>30.10035595361121</v>
+        <v>10.33324135756238</v>
       </c>
       <c r="K22" t="n">
-        <v>0.9540164308289075</v>
+        <v>0.9873931207422312</v>
       </c>
       <c r="L22" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M22" t="b">
         <v>0</v>
@@ -1326,37 +1374,37 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D23" t="n">
-        <v>61.66086959838867</v>
+        <v>13.85670852661133</v>
       </c>
       <c r="E23" t="n">
-        <v>30.23070715613351</v>
+        <v>36.71420279112473</v>
       </c>
       <c r="F23" t="n">
-        <v>124.7017049711479</v>
+        <v>13.34180062631795</v>
       </c>
       <c r="G23" t="n">
-        <v>27.17207969502444</v>
+        <v>36.87865914398213</v>
       </c>
       <c r="H23" t="n">
-        <v>74.82287154751958</v>
+        <v>4.718564380736361</v>
       </c>
       <c r="I23" t="n">
-        <v>29.39045989359219</v>
+        <v>41.39270475869747</v>
       </c>
       <c r="J23" t="n">
-        <v>31.25599141528556</v>
+        <v>13.06408850792385</v>
       </c>
       <c r="K23" t="n">
-        <v>0.9512403441792492</v>
+        <v>0.9843217034262717</v>
       </c>
       <c r="L23" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -1367,37 +1415,37 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D24" t="n">
-        <v>63.72140884399414</v>
+        <v>16.11751174926758</v>
       </c>
       <c r="E24" t="n">
-        <v>30.08794991629453</v>
+        <v>36.05782365394712</v>
       </c>
       <c r="F24" t="n">
-        <v>131.3733583691446</v>
+        <v>17.0855877232591</v>
       </c>
       <c r="G24" t="n">
-        <v>26.94573058706407</v>
+        <v>35.80450438278741</v>
       </c>
       <c r="H24" t="n">
-        <v>80.05183329486151</v>
+        <v>6.750190082205407</v>
       </c>
       <c r="I24" t="n">
-        <v>29.09709078569805</v>
+        <v>39.83764358334574</v>
       </c>
       <c r="J24" t="n">
-        <v>32.53617971949857</v>
+        <v>16.17573738121683</v>
       </c>
       <c r="K24" t="n">
-        <v>0.9489508036763983</v>
+        <v>0.9803422241552401</v>
       </c>
       <c r="L24" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M24" t="b">
         <v>0</v>
@@ -1408,37 +1456,37 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D25" t="n">
-        <v>64.94656372070312</v>
+        <v>18.35416030883789</v>
       </c>
       <c r="E25" t="n">
-        <v>30.00524208590591</v>
+        <v>35.49345840269793</v>
       </c>
       <c r="F25" t="n">
-        <v>133.3197829025517</v>
+        <v>21.35072867856308</v>
       </c>
       <c r="G25" t="n">
-        <v>26.88185763082393</v>
+        <v>34.83667659226834</v>
       </c>
       <c r="H25" t="n">
-        <v>81.34416252646579</v>
+        <v>9.224393473857083</v>
       </c>
       <c r="I25" t="n">
-        <v>29.02753968604347</v>
+        <v>38.48142541008819</v>
       </c>
       <c r="J25" t="n">
-        <v>33.32197788229313</v>
+        <v>19.93793732887131</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9481169732658601</v>
+        <v>0.9759659675238265</v>
       </c>
       <c r="L25" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M25" t="b">
         <v>0</v>
@@ -1449,37 +1497,37 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D26" t="n">
-        <v>65.81329345703125</v>
+        <v>20.48650741577148</v>
       </c>
       <c r="E26" t="n">
-        <v>29.94766761546311</v>
+        <v>35.01612435621679</v>
       </c>
       <c r="F26" t="n">
-        <v>135.6033906429596</v>
+        <v>26.29394239652244</v>
       </c>
       <c r="G26" t="n">
-        <v>26.80809812051338</v>
+        <v>33.93224653700617</v>
       </c>
       <c r="H26" t="n">
-        <v>83.29539657868985</v>
+        <v>12.42762635583186</v>
       </c>
       <c r="I26" t="n">
-        <v>28.92459360610188</v>
+        <v>37.18692173417239</v>
       </c>
       <c r="J26" t="n">
-        <v>33.94768194768195</v>
+        <v>24.27034533839459</v>
       </c>
       <c r="K26" t="n">
-        <v>0.9474139549630868</v>
+        <v>0.9708451391511432</v>
       </c>
       <c r="L26" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
@@ -1490,37 +1538,37 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D27" t="n">
-        <v>28.58290481567383</v>
+        <v>12.11480712890625</v>
       </c>
       <c r="E27" t="n">
-        <v>33.56973997808623</v>
+        <v>37.29763856428104</v>
       </c>
       <c r="F27" t="n">
-        <v>56.81984388740581</v>
+        <v>10.27487247356871</v>
       </c>
       <c r="G27" t="n">
-        <v>30.58580324704002</v>
+        <v>38.01303920526043</v>
       </c>
       <c r="H27" t="n">
-        <v>30.71212484466951</v>
+        <v>2.790924132057954</v>
       </c>
       <c r="I27" t="n">
-        <v>33.25770496349573</v>
+        <v>43.67332329996054</v>
       </c>
       <c r="J27" t="n">
-        <v>30.12803126077462</v>
+        <v>8.012715490891306</v>
       </c>
       <c r="K27" t="n">
-        <v>0.9750504721311603</v>
+        <v>0.9894132762153189</v>
       </c>
       <c r="L27" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M27" t="b">
         <v>0</v>
@@ -1531,37 +1579,37 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28" t="n">
-        <v>29.59228897094727</v>
+        <v>15.23437118530273</v>
       </c>
       <c r="E28" t="n">
-        <v>33.41901801621296</v>
+        <v>36.30255827900891</v>
       </c>
       <c r="F28" t="n">
-        <v>59.16085843054661</v>
+        <v>13.64598460665512</v>
       </c>
       <c r="G28" t="n">
-        <v>30.41045893836756</v>
+        <v>36.7807548382938</v>
       </c>
       <c r="H28" t="n">
-        <v>32.11705921398254</v>
+        <v>4.226842312666622</v>
       </c>
       <c r="I28" t="n">
-        <v>33.06344588445879</v>
+        <v>41.87064314604103</v>
       </c>
       <c r="J28" t="n">
-        <v>31.1705112960761</v>
+        <v>10.00167874856925</v>
       </c>
       <c r="K28" t="n">
-        <v>0.9743015643052283</v>
+        <v>0.9863023315208087</v>
       </c>
       <c r="L28" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M28" t="b">
         <v>0</v>
@@ -1572,37 +1620,37 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D29" t="n">
-        <v>30.41518783569336</v>
+        <v>18.28750991821289</v>
       </c>
       <c r="E29" t="n">
-        <v>33.29989857979432</v>
+        <v>35.50925786195297</v>
       </c>
       <c r="F29" t="n">
-        <v>60.98198821429362</v>
+        <v>17.51014032992458</v>
       </c>
       <c r="G29" t="n">
-        <v>30.27878781172749</v>
+        <v>35.69790734243763</v>
       </c>
       <c r="H29" t="n">
-        <v>32.98062087751975</v>
+        <v>6.05536339599815</v>
       </c>
       <c r="I29" t="n">
-        <v>32.94821533660603</v>
+        <v>40.30940149616576</v>
       </c>
       <c r="J29" t="n">
-        <v>32.02736713500305</v>
+        <v>12.43626357986622</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9738189911379806</v>
+        <v>0.9826974387859787</v>
       </c>
       <c r="L29" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M29" t="b">
         <v>0</v>
@@ -1613,37 +1661,37 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D30" t="n">
-        <v>31.29265975952148</v>
+        <v>21.33545684814453</v>
       </c>
       <c r="E30" t="n">
-        <v>33.17637882739564</v>
+        <v>34.83978414187976</v>
       </c>
       <c r="F30" t="n">
-        <v>63.06305888494732</v>
+        <v>22.17355739557738</v>
       </c>
       <c r="G30" t="n">
-        <v>30.13305328413615</v>
+        <v>34.67244986502605</v>
       </c>
       <c r="H30" t="n">
-        <v>34.12958498144786</v>
+        <v>8.484153148513146</v>
       </c>
       <c r="I30" t="n">
-        <v>32.79949353613677</v>
+        <v>38.84471861448438</v>
       </c>
       <c r="J30" t="n">
-        <v>32.96164969194015</v>
+        <v>15.53630059858946</v>
       </c>
       <c r="K30" t="n">
-        <v>0.9733214941625135</v>
+        <v>0.9786716672885766</v>
       </c>
       <c r="L30" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M30" t="b">
         <v>0</v>
@@ -1654,39 +1702,2909 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D31" t="n">
-        <v>32.479736328125</v>
+        <v>24.30652618408203</v>
       </c>
       <c r="E31" t="n">
-        <v>33.01467865905458</v>
+        <v>34.27357465656237</v>
       </c>
       <c r="F31" t="n">
-        <v>66.64772492843456</v>
+        <v>27.74980936945576</v>
       </c>
       <c r="G31" t="n">
-        <v>29.89295031842572</v>
+        <v>33.69820356835443</v>
       </c>
       <c r="H31" t="n">
-        <v>37.01380479583455</v>
+        <v>11.66171722719392</v>
       </c>
       <c r="I31" t="n">
-        <v>32.44716630625425</v>
+        <v>37.46317854408695</v>
       </c>
       <c r="J31" t="n">
-        <v>34.11556480999479</v>
+        <v>19.15837170211211</v>
       </c>
       <c r="K31" t="n">
-        <v>0.9715391667914381</v>
+        <v>0.9741086940680017</v>
       </c>
       <c r="L31" t="n">
+        <v>31</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="n">
+        <v>11.19894027709961</v>
+      </c>
+      <c r="E32" t="n">
+        <v>37.63903432267594</v>
+      </c>
+      <c r="F32" t="n">
+        <v>10.61422680716237</v>
+      </c>
+      <c r="G32" t="n">
+        <v>37.87191997374179</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3.540009118359773</v>
+      </c>
+      <c r="I32" t="n">
+        <v>42.6407598018443</v>
+      </c>
+      <c r="J32" t="n">
+        <v>10.7502152962887</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.9873992360296937</v>
+      </c>
+      <c r="L32" t="n">
+        <v>27</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="n">
+        <v>13.54910278320312</v>
+      </c>
+      <c r="E33" t="n">
+        <v>36.81169823532402</v>
+      </c>
+      <c r="F33" t="n">
+        <v>13.88801164443458</v>
+      </c>
+      <c r="G33" t="n">
+        <v>36.70440288900156</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5.2509567546797</v>
+      </c>
+      <c r="I33" t="n">
+        <v>40.92841919286493</v>
+      </c>
+      <c r="J33" t="n">
+        <v>13.41438952000819</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.9840614045377601</v>
+      </c>
+      <c r="L33" t="n">
+        <v>28</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="n">
+        <v>15.83354187011719</v>
+      </c>
+      <c r="E34" t="n">
+        <v>36.13502286018826</v>
+      </c>
+      <c r="F34" t="n">
+        <v>17.72667156085055</v>
+      </c>
+      <c r="G34" t="n">
+        <v>35.6445316268698</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7.352850432448511</v>
+      </c>
+      <c r="I34" t="n">
+        <v>39.46624628980616</v>
+      </c>
+      <c r="J34" t="n">
+        <v>16.72903637523931</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.9803259567447008</v>
+      </c>
+      <c r="L34" t="n">
+        <v>29</v>
+      </c>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="n">
+        <v>18.16559219360352</v>
+      </c>
+      <c r="E35" t="n">
+        <v>35.53830800550703</v>
+      </c>
+      <c r="F35" t="n">
+        <v>22.06815482966958</v>
+      </c>
+      <c r="G35" t="n">
+        <v>34.69314338571367</v>
+      </c>
+      <c r="H35" t="n">
+        <v>9.902224355978353</v>
+      </c>
+      <c r="I35" t="n">
+        <v>38.17347598894708</v>
+      </c>
+      <c r="J35" t="n">
+        <v>21.00008010894817</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.9763181986713579</v>
+      </c>
+      <c r="L35" t="n">
+        <v>30</v>
+      </c>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="M31" t="b">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="n">
+        <v>20.22214889526367</v>
+      </c>
+      <c r="E36" t="n">
+        <v>35.07253057102165</v>
+      </c>
+      <c r="F36" t="n">
+        <v>26.94045209515378</v>
+      </c>
+      <c r="G36" t="n">
+        <v>33.82675481404361</v>
+      </c>
+      <c r="H36" t="n">
+        <v>13.11750087193663</v>
+      </c>
+      <c r="I36" t="n">
+        <v>36.95229259129437</v>
+      </c>
+      <c r="J36" t="n">
+        <v>25.63755501222494</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.9718947307535075</v>
+      </c>
+      <c r="L36" t="n">
+        <v>31</v>
+      </c>
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="n">
+        <v>10.71938705444336</v>
+      </c>
+      <c r="E37" t="n">
+        <v>37.82910408205522</v>
+      </c>
+      <c r="F37" t="n">
+        <v>10.80095591912577</v>
+      </c>
+      <c r="G37" t="n">
+        <v>37.79618167230048</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4.034952248779133</v>
+      </c>
+      <c r="I37" t="n">
+        <v>42.07241961392086</v>
+      </c>
+      <c r="J37" t="n">
+        <v>14.42174176156682</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.9863916559868137</v>
+      </c>
+      <c r="L37" t="n">
+        <v>27</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="n">
+        <v>12.429931640625</v>
+      </c>
+      <c r="E38" t="n">
+        <v>37.1861162065595</v>
+      </c>
+      <c r="F38" t="n">
+        <v>13.73071571000115</v>
+      </c>
+      <c r="G38" t="n">
+        <v>36.75387185553728</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5.651726795826468</v>
+      </c>
+      <c r="I38" t="n">
+        <v>40.60899200956207</v>
+      </c>
+      <c r="J38" t="n">
+        <v>17.88036286747152</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.9833816084308387</v>
+      </c>
+      <c r="L38" t="n">
+        <v>28</v>
+      </c>
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="n">
+        <v>14.14228820800781</v>
+      </c>
+      <c r="E39" t="n">
+        <v>36.62560677311377</v>
+      </c>
+      <c r="F39" t="n">
+        <v>17.24771568700613</v>
+      </c>
+      <c r="G39" t="n">
+        <v>35.7634877625401</v>
+      </c>
+      <c r="H39" t="n">
+        <v>7.760857629300971</v>
+      </c>
+      <c r="I39" t="n">
+        <v>39.23170644365876</v>
+      </c>
+      <c r="J39" t="n">
+        <v>22.38633646456021</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.9799998581672736</v>
+      </c>
+      <c r="L39" t="n">
+        <v>29</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="n">
+        <v>15.68279266357422</v>
+      </c>
+      <c r="E40" t="n">
+        <v>36.17656960020287</v>
+      </c>
+      <c r="F40" t="n">
+        <v>21.17971882640881</v>
+      </c>
+      <c r="G40" t="n">
+        <v>34.87160170580376</v>
+      </c>
+      <c r="H40" t="n">
+        <v>10.39130653167996</v>
+      </c>
+      <c r="I40" t="n">
+        <v>37.96410204665322</v>
+      </c>
+      <c r="J40" t="n">
+        <v>27.42092050209205</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.9762048012096173</v>
+      </c>
+      <c r="L40" t="n">
+        <v>30</v>
+      </c>
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="n">
+        <v>17.24118041992188</v>
+      </c>
+      <c r="E41" t="n">
+        <v>35.76513364326509</v>
+      </c>
+      <c r="F41" t="n">
+        <v>25.54302606719618</v>
+      </c>
+      <c r="G41" t="n">
+        <v>34.05808014282111</v>
+      </c>
+      <c r="H41" t="n">
+        <v>13.43888051397597</v>
+      </c>
+      <c r="I41" t="n">
+        <v>36.84717268255194</v>
+      </c>
+      <c r="J41" t="n">
+        <v>33.44953426055888</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.972020304309965</v>
+      </c>
+      <c r="L41" t="n">
+        <v>31</v>
+      </c>
+      <c r="M41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="n">
+        <v>9.943073272705078</v>
+      </c>
+      <c r="E42" t="n">
+        <v>38.15559721029346</v>
+      </c>
+      <c r="F42" t="n">
+        <v>11.11395338083492</v>
+      </c>
+      <c r="G42" t="n">
+        <v>37.6721179012888</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4.660410828480852</v>
+      </c>
+      <c r="I42" t="n">
+        <v>41.44656158195534</v>
+      </c>
+      <c r="J42" t="n">
+        <v>17.81595759140954</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.9848176661617696</v>
+      </c>
+      <c r="L42" t="n">
+        <v>27</v>
+      </c>
+      <c r="M42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="n">
+        <v>11.35239028930664</v>
+      </c>
+      <c r="E43" t="n">
+        <v>37.57993047342161</v>
+      </c>
+      <c r="F43" t="n">
+        <v>14.12452248544636</v>
+      </c>
+      <c r="G43" t="n">
+        <v>36.63106586531561</v>
+      </c>
+      <c r="H43" t="n">
+        <v>6.546913588602363</v>
+      </c>
+      <c r="I43" t="n">
+        <v>39.97043752073732</v>
+      </c>
+      <c r="J43" t="n">
+        <v>22.21182850364345</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.981524319212836</v>
+      </c>
+      <c r="L43" t="n">
+        <v>28</v>
+      </c>
+      <c r="M43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="n">
+        <v>12.61641311645508</v>
+      </c>
+      <c r="E44" t="n">
+        <v>37.12144459616547</v>
+      </c>
+      <c r="F44" t="n">
+        <v>17.48122084536248</v>
+      </c>
+      <c r="G44" t="n">
+        <v>35.70508601454561</v>
+      </c>
+      <c r="H44" t="n">
+        <v>8.775172402565797</v>
+      </c>
+      <c r="I44" t="n">
+        <v>38.69824703223213</v>
+      </c>
+      <c r="J44" t="n">
+        <v>27.17644619531412</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.9780343056837606</v>
+      </c>
+      <c r="L44" t="n">
+        <v>29</v>
+      </c>
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="n">
+        <v>13.86918258666992</v>
+      </c>
+      <c r="E45" t="n">
+        <v>36.71029495220711</v>
+      </c>
+      <c r="F45" t="n">
+        <v>21.0744281886428</v>
+      </c>
+      <c r="G45" t="n">
+        <v>34.89324561100721</v>
+      </c>
+      <c r="H45" t="n">
+        <v>11.32438402558897</v>
+      </c>
+      <c r="I45" t="n">
+        <v>37.59065772396119</v>
+      </c>
+      <c r="J45" t="n">
+        <v>33.06559031281534</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.9741021960327411</v>
+      </c>
+      <c r="L45" t="n">
+        <v>30</v>
+      </c>
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="n">
+        <v>15.20344924926758</v>
+      </c>
+      <c r="E46" t="n">
+        <v>36.31138232134705</v>
+      </c>
+      <c r="F46" t="n">
+        <v>25.45868938816376</v>
+      </c>
+      <c r="G46" t="n">
+        <v>34.07244318429265</v>
+      </c>
+      <c r="H46" t="n">
+        <v>14.67068332275822</v>
+      </c>
+      <c r="I46" t="n">
+        <v>36.46630018231723</v>
+      </c>
+      <c r="J46" t="n">
+        <v>40.2988470407379</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.9692137854451718</v>
+      </c>
+      <c r="L46" t="n">
+        <v>31</v>
+      </c>
+      <c r="M46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="n">
+        <v>11.72560882568359</v>
+      </c>
+      <c r="E47" t="n">
+        <v>37.43944959137909</v>
+      </c>
+      <c r="F47" t="n">
+        <v>10.67895661827698</v>
+      </c>
+      <c r="G47" t="n">
+        <v>37.84551538611773</v>
+      </c>
+      <c r="H47" t="n">
+        <v>3.576233799825415</v>
+      </c>
+      <c r="I47" t="n">
+        <v>42.59654457384158</v>
+      </c>
+      <c r="J47" t="n">
+        <v>11.25129833898451</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.9860744561612401</v>
+      </c>
+      <c r="L47" t="n">
+        <v>27</v>
+      </c>
+      <c r="M47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="n">
+        <v>13.99520492553711</v>
+      </c>
+      <c r="E48" t="n">
+        <v>36.67101098838977</v>
+      </c>
+      <c r="F48" t="n">
+        <v>13.99809402360816</v>
+      </c>
+      <c r="G48" t="n">
+        <v>36.67011454573993</v>
+      </c>
+      <c r="H48" t="n">
+        <v>5.327305072705137</v>
+      </c>
+      <c r="I48" t="n">
+        <v>40.86572793124055</v>
+      </c>
+      <c r="J48" t="n">
+        <v>14.13022854678741</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.9823697535432911</v>
+      </c>
+      <c r="L48" t="n">
+        <v>28</v>
+      </c>
+      <c r="M48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="n">
+        <v>16.08545684814453</v>
+      </c>
+      <c r="E49" t="n">
+        <v>36.066469609199</v>
+      </c>
+      <c r="F49" t="n">
+        <v>17.85448503642715</v>
+      </c>
+      <c r="G49" t="n">
+        <v>35.61333032189754</v>
+      </c>
+      <c r="H49" t="n">
+        <v>7.547381681921393</v>
+      </c>
+      <c r="I49" t="n">
+        <v>39.35284047426027</v>
+      </c>
+      <c r="J49" t="n">
+        <v>17.54175588865096</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.9782041589207108</v>
+      </c>
+      <c r="L49" t="n">
+        <v>29</v>
+      </c>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="n">
+        <v>18.18566513061523</v>
+      </c>
+      <c r="E50" t="n">
+        <v>35.53351171106908</v>
+      </c>
+      <c r="F50" t="n">
+        <v>22.17407958657149</v>
+      </c>
+      <c r="G50" t="n">
+        <v>34.67234758915176</v>
+      </c>
+      <c r="H50" t="n">
+        <v>10.22076587598006</v>
+      </c>
+      <c r="I50" t="n">
+        <v>38.03596920719936</v>
+      </c>
+      <c r="J50" t="n">
+        <v>21.75107865914371</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.9737225209578777</v>
+      </c>
+      <c r="L50" t="n">
+        <v>30</v>
+      </c>
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="n">
+        <v>20.26837921142578</v>
+      </c>
+      <c r="E51" t="n">
+        <v>35.06261339736693</v>
+      </c>
+      <c r="F51" t="n">
+        <v>27.16088297483427</v>
+      </c>
+      <c r="G51" t="n">
+        <v>33.79136476523622</v>
+      </c>
+      <c r="H51" t="n">
+        <v>13.60125214388866</v>
+      </c>
+      <c r="I51" t="n">
+        <v>36.79501469104362</v>
+      </c>
+      <c r="J51" t="n">
+        <v>26.8975990149805</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.9685019619574077</v>
+      </c>
+      <c r="L51" t="n">
+        <v>31</v>
+      </c>
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="n">
+        <v>6.165256500244141</v>
+      </c>
+      <c r="E52" t="n">
+        <v>40.2312921110837</v>
+      </c>
+      <c r="F52" t="n">
+        <v>9.215793563697934</v>
+      </c>
+      <c r="G52" t="n">
+        <v>38.4854762299526</v>
+      </c>
+      <c r="H52" t="n">
+        <v>5.367592510811813</v>
+      </c>
+      <c r="I52" t="n">
+        <v>40.83300822601011</v>
+      </c>
+      <c r="J52" t="n">
+        <v>39.53310209621475</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.9846627636603253</v>
+      </c>
+      <c r="L52" t="n">
+        <v>27</v>
+      </c>
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="n">
+        <v>6.900550842285156</v>
+      </c>
+      <c r="E53" t="n">
+        <v>39.74196600823944</v>
+      </c>
+      <c r="F53" t="n">
+        <v>11.17609114711928</v>
+      </c>
+      <c r="G53" t="n">
+        <v>37.64790425838957</v>
+      </c>
+      <c r="H53" t="n">
+        <v>6.883288383857543</v>
+      </c>
+      <c r="I53" t="n">
+        <v>39.75284395629977</v>
+      </c>
+      <c r="J53" t="n">
+        <v>50.84251357641583</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.9818820069500437</v>
+      </c>
+      <c r="L53" t="n">
+        <v>28</v>
+      </c>
+      <c r="M53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="n">
+        <v>7.692153930664062</v>
+      </c>
+      <c r="E54" t="n">
+        <v>39.27032394379848</v>
+      </c>
+      <c r="F54" t="n">
+        <v>13.2798549703099</v>
+      </c>
+      <c r="G54" t="n">
+        <v>36.89887028752934</v>
+      </c>
+      <c r="H54" t="n">
+        <v>8.565465447540635</v>
+      </c>
+      <c r="I54" t="n">
+        <v>38.80329393355496</v>
+      </c>
+      <c r="J54" t="n">
+        <v>66.1812673567281</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.9787346197632851</v>
+      </c>
+      <c r="L54" t="n">
+        <v>29</v>
+      </c>
+      <c r="M54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="n">
+        <v>8.519668579101562</v>
+      </c>
+      <c r="E55" t="n">
+        <v>38.82657660123148</v>
+      </c>
+      <c r="F55" t="n">
+        <v>15.74281637054764</v>
+      </c>
+      <c r="G55" t="n">
+        <v>36.15997931143931</v>
+      </c>
+      <c r="H55" t="n">
+        <v>10.57892829784467</v>
+      </c>
+      <c r="I55" t="n">
+        <v>37.8863868729984</v>
+      </c>
+      <c r="J55" t="n">
+        <v>90.30106786083363</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.9752105853072015</v>
+      </c>
+      <c r="L55" t="n">
+        <v>30</v>
+      </c>
+      <c r="M55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="n">
+        <v>9.332080841064453</v>
+      </c>
+      <c r="E56" t="n">
+        <v>38.4310186856487</v>
+      </c>
+      <c r="F56" t="n">
+        <v>18.24016457508719</v>
+      </c>
+      <c r="G56" t="n">
+        <v>35.52051608359626</v>
+      </c>
+      <c r="H56" t="n">
+        <v>12.60912494128123</v>
+      </c>
+      <c r="I56" t="n">
+        <v>37.12395412784878</v>
+      </c>
+      <c r="J56" t="n">
+        <v>120.5814167433303</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.9714573847970391</v>
+      </c>
+      <c r="L56" t="n">
+        <v>31</v>
+      </c>
+      <c r="M56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="n">
+        <v>8.869369506835938</v>
+      </c>
+      <c r="E57" t="n">
+        <v>38.6518761244929</v>
+      </c>
+      <c r="F57" t="n">
+        <v>10.98515680049266</v>
+      </c>
+      <c r="G57" t="n">
+        <v>37.72274100512363</v>
+      </c>
+      <c r="H57" t="n">
+        <v>5.239490478516757</v>
+      </c>
+      <c r="I57" t="n">
+        <v>40.93791305397102</v>
+      </c>
+      <c r="J57" t="n">
+        <v>23.88338192419825</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.9834315149675708</v>
+      </c>
+      <c r="L57" t="n">
+        <v>27</v>
+      </c>
+      <c r="M57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="n">
+        <v>9.945201873779297</v>
+      </c>
+      <c r="E58" t="n">
+        <v>38.15466757743447</v>
+      </c>
+      <c r="F58" t="n">
+        <v>13.78304553834086</v>
+      </c>
+      <c r="G58" t="n">
+        <v>36.73735169830715</v>
+      </c>
+      <c r="H58" t="n">
+        <v>7.192856106015754</v>
+      </c>
+      <c r="I58" t="n">
+        <v>39.56178988595543</v>
+      </c>
+      <c r="J58" t="n">
+        <v>29.96273859869699</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.9799595089317258</v>
+      </c>
+      <c r="L58" t="n">
+        <v>28</v>
+      </c>
+      <c r="M58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="n">
+        <v>10.99330520629883</v>
+      </c>
+      <c r="E59" t="n">
+        <v>37.71952075446281</v>
+      </c>
+      <c r="F59" t="n">
+        <v>16.82964683901854</v>
+      </c>
+      <c r="G59" t="n">
+        <v>35.87005358229859</v>
+      </c>
+      <c r="H59" t="n">
+        <v>9.410693634125996</v>
+      </c>
+      <c r="I59" t="n">
+        <v>38.39458725711503</v>
+      </c>
+      <c r="J59" t="n">
+        <v>37.68060945809975</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.9761579357901953</v>
+      </c>
+      <c r="L59" t="n">
+        <v>29</v>
+      </c>
+      <c r="M59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="n">
+        <v>11.81134414672852</v>
+      </c>
+      <c r="E60" t="n">
+        <v>37.4078103715027</v>
+      </c>
+      <c r="F60" t="n">
+        <v>19.57812665164064</v>
+      </c>
+      <c r="G60" t="n">
+        <v>35.21309227219901</v>
+      </c>
+      <c r="H60" t="n">
+        <v>11.53784292417373</v>
+      </c>
+      <c r="I60" t="n">
+        <v>37.50955738676792</v>
+      </c>
+      <c r="J60" t="n">
+        <v>45.34578792596437</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.9728697749269264</v>
+      </c>
+      <c r="L60" t="n">
+        <v>30</v>
+      </c>
+      <c r="M60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="n">
+        <v>12.8516731262207</v>
+      </c>
+      <c r="E61" t="n">
+        <v>37.04120689839966</v>
+      </c>
+      <c r="F61" t="n">
+        <v>23.21586000047871</v>
+      </c>
+      <c r="G61" t="n">
+        <v>34.47295584709592</v>
+      </c>
+      <c r="H61" t="n">
+        <v>14.42248796689059</v>
+      </c>
+      <c r="I61" t="n">
+        <v>36.54040175582345</v>
+      </c>
+      <c r="J61" t="n">
+        <v>55.94195475885617</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.9684849415617496</v>
+      </c>
+      <c r="L61" t="n">
+        <v>31</v>
+      </c>
+      <c r="M61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" t="n">
+        <v>4.562973022460938</v>
+      </c>
+      <c r="E62" t="n">
+        <v>41.53832459754901</v>
+      </c>
+      <c r="F62" t="n">
+        <v>8.183750501622677</v>
+      </c>
+      <c r="G62" t="n">
+        <v>39.00127980317792</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1.742500445747331</v>
+      </c>
+      <c r="I62" t="n">
+        <v>45.71907463001403</v>
+      </c>
+      <c r="J62" t="n">
+        <v>10.89497527118574</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.9956440133742098</v>
+      </c>
+      <c r="L62" t="n">
+        <v>27</v>
+      </c>
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" t="n">
+        <v>5.431205749511719</v>
+      </c>
+      <c r="E63" t="n">
+        <v>40.7818410545421</v>
+      </c>
+      <c r="F63" t="n">
+        <v>10.51512098508563</v>
+      </c>
+      <c r="G63" t="n">
+        <v>37.9126608690284</v>
+      </c>
+      <c r="H63" t="n">
+        <v>2.637027713386906</v>
+      </c>
+      <c r="I63" t="n">
+        <v>43.91965666907709</v>
+      </c>
+      <c r="J63" t="n">
+        <v>11.89185265831972</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.9945316167142731</v>
+      </c>
+      <c r="L63" t="n">
+        <v>28</v>
+      </c>
+      <c r="M63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="n">
+        <v>6.543361663818359</v>
+      </c>
+      <c r="E64" t="n">
+        <v>39.97279435639118</v>
+      </c>
+      <c r="F64" t="n">
+        <v>13.28569573792856</v>
+      </c>
+      <c r="G64" t="n">
+        <v>36.89696058634106</v>
+      </c>
+      <c r="H64" t="n">
+        <v>3.777770382471307</v>
+      </c>
+      <c r="I64" t="n">
+        <v>42.35844803432492</v>
+      </c>
+      <c r="J64" t="n">
+        <v>13.09999500274849</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.9931149262569933</v>
+      </c>
+      <c r="L64" t="n">
+        <v>29</v>
+      </c>
+      <c r="M64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="n">
+        <v>7.810569763183594</v>
+      </c>
+      <c r="E65" t="n">
+        <v>39.20397645046803</v>
+      </c>
+      <c r="F65" t="n">
+        <v>16.51627795107784</v>
+      </c>
+      <c r="G65" t="n">
+        <v>35.95168177897771</v>
+      </c>
+      <c r="H65" t="n">
+        <v>5.243987745609132</v>
+      </c>
+      <c r="I65" t="n">
+        <v>40.93418692727924</v>
+      </c>
+      <c r="J65" t="n">
+        <v>14.45195435250014</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.9915013190081842</v>
+      </c>
+      <c r="L65" t="n">
+        <v>30</v>
+      </c>
+      <c r="M65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" t="n">
+        <v>9.475162506103516</v>
+      </c>
+      <c r="E66" t="n">
+        <v>38.36493693689667</v>
+      </c>
+      <c r="F66" t="n">
+        <v>20.87652796633883</v>
+      </c>
+      <c r="G66" t="n">
+        <v>34.93422089260069</v>
+      </c>
+      <c r="H66" t="n">
+        <v>7.422470214769685</v>
+      </c>
+      <c r="I66" t="n">
+        <v>39.42531897353229</v>
+      </c>
+      <c r="J66" t="n">
+        <v>16.11309853094843</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.9893083601161965</v>
+      </c>
+      <c r="L66" t="n">
+        <v>31</v>
+      </c>
+      <c r="M66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" t="n">
+        <v>4.209747314453125</v>
+      </c>
+      <c r="E67" t="n">
+        <v>41.88824332308278</v>
+      </c>
+      <c r="F67" t="n">
+        <v>8.155138650204037</v>
+      </c>
+      <c r="G67" t="n">
+        <v>39.01649011738501</v>
+      </c>
+      <c r="H67" t="n">
+        <v>2.168836417453393</v>
+      </c>
+      <c r="I67" t="n">
+        <v>44.76853563891262</v>
+      </c>
+      <c r="J67" t="n">
+        <v>12.29510810937573</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.9949492530054262</v>
+      </c>
+      <c r="L67" t="n">
+        <v>27</v>
+      </c>
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" t="n">
+        <v>5.013935089111328</v>
+      </c>
+      <c r="E68" t="n">
+        <v>41.12901653627691</v>
+      </c>
+      <c r="F68" t="n">
+        <v>10.27781602480411</v>
+      </c>
+      <c r="G68" t="n">
+        <v>38.0117952141713</v>
+      </c>
+      <c r="H68" t="n">
+        <v>3.112338128379143</v>
+      </c>
+      <c r="I68" t="n">
+        <v>43.1999358768133</v>
+      </c>
+      <c r="J68" t="n">
+        <v>13.45225021809411</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.9937129718614494</v>
+      </c>
+      <c r="L68" t="n">
+        <v>28</v>
+      </c>
+      <c r="M68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" t="n">
+        <v>6.062950134277344</v>
+      </c>
+      <c r="E69" t="n">
+        <v>40.30396364544085</v>
+      </c>
+      <c r="F69" t="n">
+        <v>13.09884538520326</v>
+      </c>
+      <c r="G69" t="n">
+        <v>36.95847344978136</v>
+      </c>
+      <c r="H69" t="n">
+        <v>4.456898928380159</v>
+      </c>
+      <c r="I69" t="n">
+        <v>41.64047575411863</v>
+      </c>
+      <c r="J69" t="n">
+        <v>14.91403538715367</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.9920958033738188</v>
+      </c>
+      <c r="L69" t="n">
+        <v>29</v>
+      </c>
+      <c r="M69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" t="n">
+        <v>7.254535675048828</v>
+      </c>
+      <c r="E70" t="n">
+        <v>39.52470740126873</v>
+      </c>
+      <c r="F70" t="n">
+        <v>16.30323762278101</v>
+      </c>
+      <c r="G70" t="n">
+        <v>36.00806502348384</v>
+      </c>
+      <c r="H70" t="n">
+        <v>6.130060164739893</v>
+      </c>
+      <c r="I70" t="n">
+        <v>40.25615623855806</v>
+      </c>
+      <c r="J70" t="n">
+        <v>16.50884816424208</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.990195825280874</v>
+      </c>
+      <c r="L70" t="n">
+        <v>30</v>
+      </c>
+      <c r="M70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" t="n">
+        <v>8.740879058837891</v>
+      </c>
+      <c r="E71" t="n">
+        <v>38.71525249605951</v>
+      </c>
+      <c r="F71" t="n">
+        <v>20.52629820229711</v>
+      </c>
+      <c r="G71" t="n">
+        <v>35.00769726902761</v>
+      </c>
+      <c r="H71" t="n">
+        <v>8.578048579987344</v>
+      </c>
+      <c r="I71" t="n">
+        <v>38.79691859421758</v>
+      </c>
+      <c r="J71" t="n">
+        <v>18.4686487248133</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.9877492736701259</v>
+      </c>
+      <c r="L71" t="n">
+        <v>31</v>
+      </c>
+      <c r="M71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" t="n">
+        <v>4.54541015625</v>
+      </c>
+      <c r="E72" t="n">
+        <v>41.55507282867875</v>
+      </c>
+      <c r="F72" t="n">
+        <v>8.21737777730725</v>
+      </c>
+      <c r="G72" t="n">
+        <v>38.98347107625752</v>
+      </c>
+      <c r="H72" t="n">
+        <v>2.06029030505702</v>
+      </c>
+      <c r="I72" t="n">
+        <v>44.9915194195438</v>
+      </c>
+      <c r="J72" t="n">
+        <v>11.30320800275957</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.9947130744680265</v>
+      </c>
+      <c r="L72" t="n">
+        <v>27</v>
+      </c>
+      <c r="M72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" t="n">
+        <v>5.441131591796875</v>
+      </c>
+      <c r="E73" t="n">
+        <v>40.77391131580243</v>
+      </c>
+      <c r="F73" t="n">
+        <v>10.51987652430975</v>
+      </c>
+      <c r="G73" t="n">
+        <v>37.91069718495592</v>
+      </c>
+      <c r="H73" t="n">
+        <v>3.03307447845684</v>
+      </c>
+      <c r="I73" t="n">
+        <v>43.31197286137302</v>
+      </c>
+      <c r="J73" t="n">
+        <v>12.4197659544227</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.9933102768315485</v>
+      </c>
+      <c r="L73" t="n">
+        <v>28</v>
+      </c>
+      <c r="M73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" t="n">
+        <v>6.595436096191406</v>
+      </c>
+      <c r="E74" t="n">
+        <v>39.93836844092742</v>
+      </c>
+      <c r="F74" t="n">
+        <v>13.44433252056005</v>
+      </c>
+      <c r="G74" t="n">
+        <v>36.84541115471359</v>
+      </c>
+      <c r="H74" t="n">
+        <v>4.427418675444578</v>
+      </c>
+      <c r="I74" t="n">
+        <v>41.66929768223198</v>
+      </c>
+      <c r="J74" t="n">
+        <v>13.7702369070757</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.991423243937363</v>
+      </c>
+      <c r="L74" t="n">
+        <v>29</v>
+      </c>
+      <c r="M74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" t="n">
+        <v>7.778228759765625</v>
+      </c>
+      <c r="E75" t="n">
+        <v>39.22199649153032</v>
+      </c>
+      <c r="F75" t="n">
+        <v>16.56360077865125</v>
+      </c>
+      <c r="G75" t="n">
+        <v>35.93925606419738</v>
+      </c>
+      <c r="H75" t="n">
+        <v>6.011950575001156</v>
+      </c>
+      <c r="I75" t="n">
+        <v>40.34064959327707</v>
+      </c>
+      <c r="J75" t="n">
+        <v>15.10481129357534</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.9894348459388559</v>
+      </c>
+      <c r="L75" t="n">
+        <v>30</v>
+      </c>
+      <c r="M75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" t="n">
+        <v>9.340183258056641</v>
+      </c>
+      <c r="E76" t="n">
+        <v>38.42724963526256</v>
+      </c>
+      <c r="F76" t="n">
+        <v>20.82106195157444</v>
+      </c>
+      <c r="G76" t="n">
+        <v>34.94577484495161</v>
+      </c>
+      <c r="H76" t="n">
+        <v>8.341013070373467</v>
+      </c>
+      <c r="I76" t="n">
+        <v>38.91861559132662</v>
+      </c>
+      <c r="J76" t="n">
+        <v>16.78688524590164</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.9869203698530344</v>
+      </c>
+      <c r="L76" t="n">
+        <v>31</v>
+      </c>
+      <c r="M76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" t="n">
+        <v>6.994991302490234</v>
+      </c>
+      <c r="E77" t="n">
+        <v>39.68293182037612</v>
+      </c>
+      <c r="F77" t="n">
+        <v>8.735798926957296</v>
+      </c>
+      <c r="G77" t="n">
+        <v>38.71777731605907</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1.251217569319355</v>
+      </c>
+      <c r="I77" t="n">
+        <v>47.15747526842614</v>
+      </c>
+      <c r="J77" t="n">
+        <v>7.727162859248342</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.9966179811763584</v>
+      </c>
+      <c r="L77" t="n">
+        <v>27</v>
+      </c>
+      <c r="M77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" t="n">
+        <v>8.145366668701172</v>
+      </c>
+      <c r="E78" t="n">
+        <v>39.02169721749551</v>
+      </c>
+      <c r="F78" t="n">
+        <v>11.0212995011676</v>
+      </c>
+      <c r="G78" t="n">
+        <v>37.70847556468902</v>
+      </c>
+      <c r="H78" t="n">
+        <v>1.806783998853785</v>
+      </c>
+      <c r="I78" t="n">
+        <v>45.56174125137662</v>
+      </c>
+      <c r="J78" t="n">
+        <v>8.380294747610371</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.9958150830176191</v>
+      </c>
+      <c r="L78" t="n">
+        <v>28</v>
+      </c>
+      <c r="M78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" t="n">
+        <v>9.578540802001953</v>
+      </c>
+      <c r="E79" t="n">
+        <v>38.31781007311995</v>
+      </c>
+      <c r="F79" t="n">
+        <v>13.82184060321557</v>
+      </c>
+      <c r="G79" t="n">
+        <v>36.7251448059432</v>
+      </c>
+      <c r="H79" t="n">
+        <v>2.655094500583485</v>
+      </c>
+      <c r="I79" t="n">
+        <v>43.89000377690888</v>
+      </c>
+      <c r="J79" t="n">
+        <v>9.146366142144377</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.9947700267066757</v>
+      </c>
+      <c r="L79" t="n">
+        <v>29</v>
+      </c>
+      <c r="M79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" t="n">
+        <v>11.16928100585938</v>
+      </c>
+      <c r="E80" t="n">
+        <v>37.65055143458469</v>
+      </c>
+      <c r="F80" t="n">
+        <v>17.16266864760317</v>
+      </c>
+      <c r="G80" t="n">
+        <v>35.78495543041826</v>
+      </c>
+      <c r="H80" t="n">
+        <v>3.777821810618263</v>
+      </c>
+      <c r="I80" t="n">
+        <v>42.35838891265751</v>
+      </c>
+      <c r="J80" t="n">
+        <v>9.942878816612934</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.993524549304016</v>
+      </c>
+      <c r="L80" t="n">
+        <v>30</v>
+      </c>
+      <c r="M80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" t="n">
+        <v>13.134765625</v>
+      </c>
+      <c r="E81" t="n">
+        <v>36.94658033169296</v>
+      </c>
+      <c r="F81" t="n">
+        <v>21.44325931117574</v>
+      </c>
+      <c r="G81" t="n">
+        <v>34.81789563369704</v>
+      </c>
+      <c r="H81" t="n">
+        <v>5.344907799675548</v>
+      </c>
+      <c r="I81" t="n">
+        <v>40.85140142892338</v>
+      </c>
+      <c r="J81" t="n">
+        <v>10.85977049587804</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.9919716655224429</v>
+      </c>
+      <c r="L81" t="n">
+        <v>31</v>
+      </c>
+      <c r="M81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" t="n">
+        <v>4.314632415771484</v>
+      </c>
+      <c r="E82" t="n">
+        <v>41.78136558870477</v>
+      </c>
+      <c r="F82" t="n">
+        <v>8.254010202605944</v>
+      </c>
+      <c r="G82" t="n">
+        <v>38.96415359504037</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1.956798078515979</v>
+      </c>
+      <c r="I82" t="n">
+        <v>45.21534347632322</v>
+      </c>
+      <c r="J82" t="n">
+        <v>11.11391868402086</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.9946630899760093</v>
+      </c>
+      <c r="L82" t="n">
+        <v>27</v>
+      </c>
+      <c r="M82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" t="n">
+        <v>5.154533386230469</v>
+      </c>
+      <c r="E83" t="n">
+        <v>41.00891003946212</v>
+      </c>
+      <c r="F83" t="n">
+        <v>10.45832578429724</v>
+      </c>
+      <c r="G83" t="n">
+        <v>37.93618194581114</v>
+      </c>
+      <c r="H83" t="n">
+        <v>2.855588938881105</v>
+      </c>
+      <c r="I83" t="n">
+        <v>43.57384669817031</v>
+      </c>
+      <c r="J83" t="n">
+        <v>12.14866994160719</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.9933338397785025</v>
+      </c>
+      <c r="L83" t="n">
+        <v>28</v>
+      </c>
+      <c r="M83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" t="n">
+        <v>6.245906829833984</v>
+      </c>
+      <c r="E84" t="n">
+        <v>40.17484859294379</v>
+      </c>
+      <c r="F84" t="n">
+        <v>13.32595989727782</v>
+      </c>
+      <c r="G84" t="n">
+        <v>36.88381858885902</v>
+      </c>
+      <c r="H84" t="n">
+        <v>4.141640685282011</v>
+      </c>
+      <c r="I84" t="n">
+        <v>41.95907942594448</v>
+      </c>
+      <c r="J84" t="n">
+        <v>13.37469387755102</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.99157412533668</v>
+      </c>
+      <c r="L84" t="n">
+        <v>29</v>
+      </c>
+      <c r="M84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" t="n">
+        <v>7.510414123535156</v>
+      </c>
+      <c r="E85" t="n">
+        <v>39.37416476246224</v>
+      </c>
+      <c r="F85" t="n">
+        <v>16.65641558260575</v>
+      </c>
+      <c r="G85" t="n">
+        <v>35.91498812787614</v>
+      </c>
+      <c r="H85" t="n">
+        <v>5.771526844596645</v>
+      </c>
+      <c r="I85" t="n">
+        <v>40.51789640872583</v>
+      </c>
+      <c r="J85" t="n">
+        <v>14.74873410599752</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.9894298083649842</v>
+      </c>
+      <c r="L85" t="n">
+        <v>30</v>
+      </c>
+      <c r="M85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" t="n">
+        <v>9.074195861816406</v>
+      </c>
+      <c r="E86" t="n">
+        <v>38.55272211815357</v>
+      </c>
+      <c r="F86" t="n">
+        <v>20.89274183989079</v>
+      </c>
+      <c r="G86" t="n">
+        <v>34.93084922907857</v>
+      </c>
+      <c r="H86" t="n">
+        <v>8.060722916581469</v>
+      </c>
+      <c r="I86" t="n">
+        <v>39.06706368119485</v>
+      </c>
+      <c r="J86" t="n">
+        <v>16.40450563204005</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.9867118447611207</v>
+      </c>
+      <c r="L86" t="n">
+        <v>31</v>
+      </c>
+      <c r="M86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" t="n">
+        <v>4.195339202880859</v>
+      </c>
+      <c r="E87" t="n">
+        <v>41.9031328056996</v>
+      </c>
+      <c r="F87" t="n">
+        <v>8.344452274107999</v>
+      </c>
+      <c r="G87" t="n">
+        <v>38.91682525801033</v>
+      </c>
+      <c r="H87" t="n">
+        <v>2.517299860049659</v>
+      </c>
+      <c r="I87" t="n">
+        <v>44.12145409201841</v>
+      </c>
+      <c r="J87" t="n">
+        <v>12.49554316220983</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.9926933752910063</v>
+      </c>
+      <c r="L87" t="n">
+        <v>27</v>
+      </c>
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" t="n">
+        <v>5.067665100097656</v>
+      </c>
+      <c r="E88" t="n">
+        <v>41.08272454337918</v>
+      </c>
+      <c r="F88" t="n">
+        <v>10.68500782219524</v>
+      </c>
+      <c r="G88" t="n">
+        <v>37.84305516432867</v>
+      </c>
+      <c r="H88" t="n">
+        <v>3.653419260478256</v>
+      </c>
+      <c r="I88" t="n">
+        <v>42.50380846864579</v>
+      </c>
+      <c r="J88" t="n">
+        <v>13.78616881409414</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.9907583833437834</v>
+      </c>
+      <c r="L88" t="n">
+        <v>28</v>
+      </c>
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" t="n">
+        <v>6.130424499511719</v>
+      </c>
+      <c r="E89" t="n">
+        <v>40.25589812709616</v>
+      </c>
+      <c r="F89" t="n">
+        <v>13.47640483310809</v>
+      </c>
+      <c r="G89" t="n">
+        <v>36.83506312095179</v>
+      </c>
+      <c r="H89" t="n">
+        <v>5.141930710249535</v>
+      </c>
+      <c r="I89" t="n">
+        <v>41.01954140828481</v>
+      </c>
+      <c r="J89" t="n">
+        <v>15.3318516785589</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.9883026369039966</v>
+      </c>
+      <c r="L89" t="n">
+        <v>29</v>
+      </c>
+      <c r="M89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>30</v>
+      </c>
+      <c r="C90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" t="n">
+        <v>7.331737518310547</v>
+      </c>
+      <c r="E90" t="n">
+        <v>39.47873452366854</v>
+      </c>
+      <c r="F90" t="n">
+        <v>16.71131187382989</v>
+      </c>
+      <c r="G90" t="n">
+        <v>35.90069816587816</v>
+      </c>
+      <c r="H90" t="n">
+        <v>6.970374276755647</v>
+      </c>
+      <c r="I90" t="n">
+        <v>39.69824262545279</v>
+      </c>
+      <c r="J90" t="n">
+        <v>17.09337506520605</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.985652807740468</v>
+      </c>
+      <c r="L90" t="n">
+        <v>30</v>
+      </c>
+      <c r="M90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" t="n">
+        <v>8.837329864501953</v>
+      </c>
+      <c r="E91" t="n">
+        <v>38.66759294981679</v>
+      </c>
+      <c r="F91" t="n">
+        <v>20.95301843782948</v>
+      </c>
+      <c r="G91" t="n">
+        <v>34.91833765715143</v>
+      </c>
+      <c r="H91" t="n">
+        <v>9.552153917685215</v>
+      </c>
+      <c r="I91" t="n">
+        <v>38.32979049065155</v>
+      </c>
+      <c r="J91" t="n">
+        <v>19.23992660550459</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.9820466797640994</v>
+      </c>
+      <c r="L91" t="n">
+        <v>31</v>
+      </c>
+      <c r="M91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" t="n">
+        <v>4.685268402099609</v>
+      </c>
+      <c r="E92" t="n">
+        <v>41.42345885769637</v>
+      </c>
+      <c r="F92" t="n">
+        <v>8.283194530186767</v>
+      </c>
+      <c r="G92" t="n">
+        <v>38.94882500016696</v>
+      </c>
+      <c r="H92" t="n">
+        <v>1.446034257361542</v>
+      </c>
+      <c r="I92" t="n">
+        <v>46.52901779107981</v>
+      </c>
+      <c r="J92" t="n">
+        <v>9.87545677152006</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.9966223757070306</v>
+      </c>
+      <c r="L92" t="n">
+        <v>27</v>
+      </c>
+      <c r="M92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" t="n">
+        <v>5.580299377441406</v>
+      </c>
+      <c r="E93" t="n">
+        <v>40.66422861843758</v>
+      </c>
+      <c r="F93" t="n">
+        <v>10.49235715363352</v>
+      </c>
+      <c r="G93" t="n">
+        <v>37.92207295570613</v>
+      </c>
+      <c r="H93" t="n">
+        <v>2.131190047249166</v>
+      </c>
+      <c r="I93" t="n">
+        <v>44.84458181547213</v>
+      </c>
+      <c r="J93" t="n">
+        <v>10.73217063784492</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.9957694634846544</v>
+      </c>
+      <c r="L93" t="n">
+        <v>28</v>
+      </c>
+      <c r="M93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" t="n">
+        <v>6.700237274169922</v>
+      </c>
+      <c r="E94" t="n">
+        <v>39.86990178310653</v>
+      </c>
+      <c r="F94" t="n">
+        <v>13.27638172607086</v>
+      </c>
+      <c r="G94" t="n">
+        <v>36.90000630000969</v>
+      </c>
+      <c r="H94" t="n">
+        <v>3.148795117166624</v>
+      </c>
+      <c r="I94" t="n">
+        <v>43.14935957576151</v>
+      </c>
+      <c r="J94" t="n">
+        <v>11.71436232013585</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.9946795521090194</v>
+      </c>
+      <c r="L94" t="n">
+        <v>29</v>
+      </c>
+      <c r="M94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" t="n">
+        <v>8.041210174560547</v>
+      </c>
+      <c r="E95" t="n">
+        <v>39.0775894737028</v>
+      </c>
+      <c r="F95" t="n">
+        <v>16.67462140186232</v>
+      </c>
+      <c r="G95" t="n">
+        <v>35.9102437884596</v>
+      </c>
+      <c r="H95" t="n">
+        <v>4.4766604838684</v>
+      </c>
+      <c r="I95" t="n">
+        <v>41.62126202730553</v>
+      </c>
+      <c r="J95" t="n">
+        <v>12.8106338269071</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.9934162278491165</v>
+      </c>
+      <c r="L95" t="n">
+        <v>30</v>
+      </c>
+      <c r="M95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" t="n">
+        <v>9.629165649414062</v>
+      </c>
+      <c r="E96" t="n">
+        <v>38.29491702980516</v>
+      </c>
+      <c r="F96" t="n">
+        <v>20.79094790111873</v>
+      </c>
+      <c r="G96" t="n">
+        <v>34.95206070726402</v>
+      </c>
+      <c r="H96" t="n">
+        <v>6.262653522016656</v>
+      </c>
+      <c r="I96" t="n">
+        <v>40.16321975613772</v>
+      </c>
+      <c r="J96" t="n">
+        <v>14.09831128320964</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.9918002359893332</v>
+      </c>
+      <c r="L96" t="n">
+        <v>31</v>
+      </c>
+      <c r="M96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" t="n">
+        <v>4.165988922119141</v>
+      </c>
+      <c r="E97" t="n">
+        <v>41.933622500975</v>
+      </c>
+      <c r="F97" t="n">
+        <v>8.064727318071016</v>
+      </c>
+      <c r="G97" t="n">
+        <v>39.06490673118021</v>
+      </c>
+      <c r="H97" t="n">
+        <v>2.299811360858664</v>
+      </c>
+      <c r="I97" t="n">
+        <v>44.51388145849429</v>
+      </c>
+      <c r="J97" t="n">
+        <v>13.18897162406923</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0.9949144101878211</v>
+      </c>
+      <c r="L97" t="n">
+        <v>27</v>
+      </c>
+      <c r="M97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" t="n">
+        <v>4.940338134765625</v>
+      </c>
+      <c r="E98" t="n">
+        <v>41.19323686228219</v>
+      </c>
+      <c r="F98" t="n">
+        <v>10.19639924804882</v>
+      </c>
+      <c r="G98" t="n">
+        <v>38.0463352859502</v>
+      </c>
+      <c r="H98" t="n">
+        <v>3.310044775453683</v>
+      </c>
+      <c r="I98" t="n">
+        <v>42.93246492288284</v>
+      </c>
+      <c r="J98" t="n">
+        <v>14.49911504424779</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0.9936520168254984</v>
+      </c>
+      <c r="L98" t="n">
+        <v>28</v>
+      </c>
+      <c r="M98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" t="n">
+        <v>5.971683502197266</v>
+      </c>
+      <c r="E99" t="n">
+        <v>40.36983578709044</v>
+      </c>
+      <c r="F99" t="n">
+        <v>12.98789702311956</v>
+      </c>
+      <c r="G99" t="n">
+        <v>36.99541524282304</v>
+      </c>
+      <c r="H99" t="n">
+        <v>4.706125869295556</v>
+      </c>
+      <c r="I99" t="n">
+        <v>41.40416822301289</v>
+      </c>
+      <c r="J99" t="n">
+        <v>16.16277205746347</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.9919882293796353</v>
+      </c>
+      <c r="L99" t="n">
+        <v>29</v>
+      </c>
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" t="n">
+        <v>7.121589660644531</v>
+      </c>
+      <c r="E100" t="n">
+        <v>39.60503414451858</v>
+      </c>
+      <c r="F100" t="n">
+        <v>16.13997725612551</v>
+      </c>
+      <c r="G100" t="n">
+        <v>36.05177442473565</v>
+      </c>
+      <c r="H100" t="n">
+        <v>6.42501735560444</v>
+      </c>
+      <c r="I100" t="n">
+        <v>40.05206055723246</v>
+      </c>
+      <c r="J100" t="n">
+        <v>17.96614351312453</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.9900907643288781</v>
+      </c>
+      <c r="L100" t="n">
+        <v>30</v>
+      </c>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" t="n">
+        <v>8.563079833984375</v>
+      </c>
+      <c r="E101" t="n">
+        <v>38.80450367879965</v>
+      </c>
+      <c r="F101" t="n">
+        <v>20.35168045757646</v>
+      </c>
+      <c r="G101" t="n">
+        <v>35.04480085718416</v>
+      </c>
+      <c r="H101" t="n">
+        <v>8.922747487336464</v>
+      </c>
+      <c r="I101" t="n">
+        <v>38.62581758188775</v>
+      </c>
+      <c r="J101" t="n">
+        <v>20.18666255967965</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.9876306622019291</v>
+      </c>
+      <c r="L101" t="n">
+        <v>31</v>
+      </c>
+      <c r="M101" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>